<commit_message>
Сб 28.11.20 : 12:06:11,29
</commit_message>
<xml_diff>
--- a/first_lab.xlsx
+++ b/first_lab.xlsx
@@ -874,7 +874,7 @@
   <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+      <selection activeCell="P20" sqref="B2:P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,7 +984,7 @@
         <v>14</v>
       </c>
       <c r="P2" s="18">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="Q2" s="16"/>
     </row>
@@ -1343,7 +1343,7 @@
         <v>0</v>
       </c>
       <c r="P9" s="10" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -1606,7 +1606,7 @@
         <v>0</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="T14" t="s">
         <v>91</v>
@@ -1659,7 +1659,7 @@
         <v>0</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="T15" t="s">
         <v>95</v>

</xml_diff>